<commit_message>
Modif Bilan Massique Châssis
</commit_message>
<xml_diff>
--- a/BP_Budget Previsionnel/BM_Budget Massique/Budget massique_V4.0.xlsx
+++ b/BP_Budget Previsionnel/BM_Budget Massique/Budget massique_V4.0.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31BAA2A5-1A6A-49E5-81AE-885C36AE83F2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1175BAB0-559B-4845-B6F6-F07ADF13EC7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="47">
   <si>
     <t>Motorisation</t>
   </si>
@@ -436,6 +435,12 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -447,12 +452,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1069,6 +1068,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-969B-46E2-9670-90DD3D7C8179}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -2005,7 +2009,7 @@
                   <c:v>73.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>46.84</c:v>
+                  <c:v>49.34</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>46.2</c:v>
@@ -2320,7 +2324,7 @@
                   <c:v>73.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>64.84</c:v>
+                  <c:v>67.84</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>46.2</c:v>
@@ -2654,7 +2658,7 @@
                   <c:v>73.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>46.84</c:v>
+                  <c:v>49.34</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>60.1</c:v>
@@ -3015,7 +3019,7 @@
                   <c:v>73.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>64.84</c:v>
+                  <c:v>67.84</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>60.1</c:v>
@@ -3585,6 +3589,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-23C7-4F35-9095-16E44200FB64}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -3602,6 +3611,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-23C7-4F35-9095-16E44200FB64}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -3619,6 +3633,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-23C7-4F35-9095-16E44200FB64}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -3636,6 +3655,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-23C7-4F35-9095-16E44200FB64}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -3653,6 +3677,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-23C7-4F35-9095-16E44200FB64}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -3670,6 +3699,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-23C7-4F35-9095-16E44200FB64}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -3991,6 +4025,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-B2FE-4A5C-A448-158AAFD4B0B4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -4008,6 +4047,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-B2FE-4A5C-A448-158AAFD4B0B4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -4091,6 +4135,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-B2FE-4A5C-A448-158AAFD4B0B4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:dLbl>
@@ -4250,7 +4299,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>33</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5</c:v>
@@ -4610,6 +4659,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-9C41-4A7E-BE33-9A7B7D2716C5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -4627,6 +4681,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-9C41-4A7E-BE33-9A7B7D2716C5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:dLbl>
@@ -4792,7 +4851,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5</c:v>
@@ -11030,8 +11089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11063,10 +11122,10 @@
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="23"/>
+      <c r="D4" s="25"/>
       <c r="E4" s="4" t="s">
         <v>3</v>
       </c>
@@ -11221,14 +11280,14 @@
       <c r="B16" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="23"/>
-      <c r="E16" s="22" t="s">
+      <c r="D16" s="25"/>
+      <c r="E16" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="F16" s="23"/>
+      <c r="F16" s="25"/>
     </row>
     <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
@@ -11266,11 +11325,11 @@
       <c r="C19" s="5">
         <v>31.5</v>
       </c>
-      <c r="D19" s="24">
+      <c r="D19" s="26">
         <v>37</v>
       </c>
       <c r="E19" s="6">
-        <v>33</v>
+        <v>32.5</v>
       </c>
       <c r="F19" s="6">
         <v>35</v>
@@ -11286,9 +11345,13 @@
       <c r="C20" s="5">
         <v>3</v>
       </c>
-      <c r="D20" s="25"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="6">
+        <v>3</v>
+      </c>
+      <c r="F20" s="6">
+        <v>3</v>
+      </c>
     </row>
     <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
@@ -11307,12 +11370,12 @@
         <v>37</v>
       </c>
       <c r="E21" s="2">
-        <f t="shared" si="1"/>
-        <v>33</v>
+        <f>E19+E20</f>
+        <v>35.5</v>
       </c>
       <c r="F21" s="2">
-        <f t="shared" si="1"/>
-        <v>35</v>
+        <f>F19+F20</f>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -11475,11 +11538,11 @@
       </c>
       <c r="E29" s="8">
         <f t="shared" si="2"/>
-        <v>46.84</v>
+        <v>49.34</v>
       </c>
       <c r="F29" s="8">
         <f t="shared" si="2"/>
-        <v>64.84</v>
+        <v>67.84</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -11498,14 +11561,14 @@
       <c r="B33" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C33" s="22" t="s">
+      <c r="C33" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D33" s="23"/>
-      <c r="E33" s="22" t="s">
+      <c r="D33" s="25"/>
+      <c r="E33" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="F33" s="23"/>
+      <c r="F33" s="25"/>
     </row>
     <row r="34" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="2"/>
@@ -11557,10 +11620,10 @@
       <c r="D36" s="12">
         <v>23.6</v>
       </c>
-      <c r="E36" s="26">
+      <c r="E36" s="22">
         <v>22</v>
       </c>
-      <c r="F36" s="26">
+      <c r="F36" s="22">
         <v>17</v>
       </c>
     </row>
@@ -11577,10 +11640,10 @@
       <c r="D37" s="12">
         <v>5.4</v>
       </c>
-      <c r="E37" s="26">
+      <c r="E37" s="22">
         <v>5</v>
       </c>
-      <c r="F37" s="26">
+      <c r="F37" s="22">
         <v>4.5</v>
       </c>
     </row>
@@ -11597,10 +11660,10 @@
       <c r="D38" s="12">
         <v>3.3</v>
       </c>
-      <c r="E38" s="26">
+      <c r="E38" s="22">
         <v>3</v>
       </c>
-      <c r="F38" s="26">
+      <c r="F38" s="22">
         <v>3</v>
       </c>
     </row>
@@ -11617,10 +11680,10 @@
       <c r="D39" s="12">
         <v>2.6</v>
       </c>
-      <c r="E39" s="26">
+      <c r="E39" s="22">
         <v>2.6</v>
       </c>
-      <c r="F39" s="26">
+      <c r="F39" s="22">
         <v>2.6</v>
       </c>
     </row>
@@ -11637,10 +11700,10 @@
       <c r="D40" s="12">
         <v>3.8</v>
       </c>
-      <c r="E40" s="26">
+      <c r="E40" s="22">
         <v>3.5</v>
       </c>
-      <c r="F40" s="26">
+      <c r="F40" s="22">
         <v>3.5</v>
       </c>
     </row>
@@ -11657,10 +11720,10 @@
       <c r="D41" s="12">
         <v>1.9</v>
       </c>
-      <c r="E41" s="26">
+      <c r="E41" s="22">
         <v>2</v>
       </c>
-      <c r="F41" s="26">
+      <c r="F41" s="22">
         <v>2</v>
       </c>
     </row>
@@ -11702,10 +11765,10 @@
       <c r="B46" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C46" s="22" t="s">
+      <c r="C46" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D46" s="23"/>
+      <c r="D46" s="25"/>
       <c r="E46" s="3" t="s">
         <v>3</v>
       </c>
@@ -11821,10 +11884,10 @@
       <c r="B57" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C57" s="22" t="s">
+      <c r="C57" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D57" s="23"/>
+      <c r="D57" s="25"/>
       <c r="E57" s="3" t="s">
         <v>3</v>
       </c>
@@ -11919,19 +11982,19 @@
       </c>
       <c r="E61" s="6">
         <f>E29</f>
-        <v>46.84</v>
+        <v>49.34</v>
       </c>
       <c r="F61" s="6">
         <f>F29</f>
-        <v>64.84</v>
+        <v>67.84</v>
       </c>
       <c r="G61" s="6">
         <f>E29</f>
-        <v>46.84</v>
+        <v>49.34</v>
       </c>
       <c r="H61" s="6">
         <f>F29</f>
-        <v>64.84</v>
+        <v>67.84</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -11997,7 +12060,7 @@
       </c>
     </row>
     <row r="64" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="27" t="s">
+      <c r="A64" s="23" t="s">
         <v>43</v>
       </c>
       <c r="B64" s="6">
@@ -12040,19 +12103,19 @@
       </c>
       <c r="E65" s="8">
         <f t="shared" si="4"/>
-        <v>180.94</v>
+        <v>183.44</v>
       </c>
       <c r="F65" s="8">
         <f t="shared" si="4"/>
-        <v>198.94</v>
+        <v>201.94</v>
       </c>
       <c r="G65" s="8">
         <f t="shared" si="4"/>
-        <v>194.84</v>
+        <v>197.34</v>
       </c>
       <c r="H65" s="8">
         <f t="shared" si="4"/>
-        <v>212.84</v>
+        <v>215.84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>